<commit_message>
Test out spider chart.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e4496760ebc897a6/Documents/Projects/Exploration/dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e4496760ebc897a6/Documents/Projects/Experience_Monitoring_Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="8_{1BB9FD8C-FACB-4661-A21D-B6AE6F3ED951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B793C417-0F87-4E8A-8838-311686274CB7}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="8_{1BB9FD8C-FACB-4661-A21D-B6AE6F3ED951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2522E98-B814-42F6-B806-F85891045533}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{781ECAF7-DF32-4E23-B6CB-22DBBAA1EBDE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{781ECAF7-DF32-4E23-B6CB-22DBBAA1EBDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,10 +98,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -147,13 +148,14 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -496,12 +498,12 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -524,14 +526,14 @@
       </c>
       <c r="C2" s="1">
         <f ca="1">Sheet3!D2</f>
-        <v>0.85034831945352118</v>
+        <v>0.85616631084063899</v>
       </c>
       <c r="D2" s="1">
         <f ca="1">Sheet2!D2</f>
-        <v>0.98584614128062042</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.93816932062549607</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -543,10 +545,10 @@
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D6" ca="1" si="0">C3+RANDBETWEEN(5,20)/100</f>
-        <v>0.96000000000000019</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.83000000000000018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -558,10 +560,10 @@
       </c>
       <c r="D4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.07</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -573,10 +575,10 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97977011494252875</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.9197701149425288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -588,7 +590,7 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93647058823529405</v>
+        <v>0.91647058823529415</v>
       </c>
     </row>
   </sheetData>
@@ -601,25 +603,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D062291-4B99-4002-9C48-24DFD9D306E6}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -654,41 +656,41 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2">
         <f ca="1">SUM(B3:B6)</f>
-        <v>7782663</v>
+        <v>7410466</v>
       </c>
       <c r="C2" s="2">
         <f ca="1">SUM(C3:C6)</f>
-        <v>7672508.2874374576</v>
+        <v>6952271.8527383376</v>
       </c>
       <c r="D2" s="1">
         <f ca="1">C2/B2</f>
-        <v>0.98584614128062042</v>
+        <v>0.93816932062549607</v>
       </c>
       <c r="E2" s="2">
         <f ca="1">SUM(E3:E6)</f>
-        <v>25931907.5</v>
+        <v>22406483.399999999</v>
       </c>
       <c r="F2" s="2">
         <f ca="1">SUM(F3:F6)</f>
-        <v>21608615.810426865</v>
+        <v>18337100.544757269</v>
       </c>
       <c r="G2" s="1">
         <f ca="1">F2/E2</f>
-        <v>0.83328292800777826</v>
+        <v>0.81838368910479142</v>
       </c>
       <c r="H2">
         <f ca="1">SUM(H3:H6)</f>
-        <v>26786</v>
+        <v>25832</v>
       </c>
       <c r="I2" s="5">
         <f ca="1">C2/H2</f>
-        <v>286.43725406695506</v>
+        <v>269.13409154298301</v>
       </c>
       <c r="J2" s="4">
         <f>MAX(J3:J6)</f>
@@ -699,41 +701,41 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2">
         <f t="shared" ref="B3:B6" ca="1" si="0">RANDBETWEEN(1000000,3000000)</f>
-        <v>1354528</v>
+        <v>1008416</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">VLOOKUP(A3,Sheet1!$A$1:$D$6,4,FALSE)*B3</f>
-        <v>1300346.8800000004</v>
+        <v>836985.28000000014</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D6" ca="1" si="1">C3/B3</f>
-        <v>0.9600000000000003</v>
+        <v>0.83000000000000018</v>
       </c>
       <c r="E3" s="3">
         <f ca="1">B3*RANDBETWEEN(25,35)/10</f>
-        <v>4740848</v>
+        <v>2823564.8</v>
       </c>
       <c r="F3" s="3">
         <f ca="1">AVERAGE(Sheet1!B3:D3)*E3</f>
-        <v>3539833.1733333333</v>
+        <v>1985907.2426666669</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G6" ca="1" si="2">F3/E3</f>
-        <v>0.7466666666666667</v>
+        <v>0.70333333333333348</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H5" ca="1" si="3">RANDBETWEEN(5000,10000)</f>
-        <v>6270</v>
+        <v>8595</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" ref="I3:I6" ca="1" si="4">C3/H3</f>
-        <v>207.39184688995221</v>
+        <v>97.380486329261217</v>
       </c>
       <c r="J3" s="4">
         <v>44732</v>
@@ -743,41 +745,41 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1692448</v>
+        <v>2889828</v>
       </c>
       <c r="C4" s="2">
         <f ca="1">VLOOKUP(A4,Sheet1!$A$1:$D$6,4,FALSE)*B4</f>
-        <v>1810919.36</v>
+        <v>2889828</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.07</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" ref="E4:E6" ca="1" si="6">B4*RANDBETWEEN(25,35)/10</f>
-        <v>4908099.2</v>
+        <v>8091518.4000000004</v>
       </c>
       <c r="F4" s="3">
         <f ca="1">AVERAGE(Sheet1!B4:D4)*E4</f>
-        <v>4171884.32</v>
+        <v>6688988.5440000007</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85</v>
+        <v>0.82666666666666666</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="3"/>
-        <v>6059</v>
+        <v>6696</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>298.88089783792708</v>
+        <v>431.57526881720429</v>
       </c>
       <c r="J4" s="4">
         <v>45137</v>
@@ -787,81 +789,84 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2919442</v>
+        <v>2003442</v>
       </c>
       <c r="C5" s="2">
         <f ca="1">VLOOKUP(A5,Sheet1!$A$1:$D$6,4,FALSE)*B5</f>
-        <v>2860382.0239080461</v>
+        <v>1842706.0786206897</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97977011494252875</v>
+        <v>0.9197701149425288</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>9926102.8000000007</v>
+        <v>6210670.2000000002</v>
       </c>
       <c r="F5" s="3">
         <f ca="1">AVERAGE(Sheet1!B5:D5)*E5</f>
-        <v>8402579.1288582385</v>
+        <v>5133202.2051494261</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.84651340996168589</v>
+        <v>0.82651340996168599</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="3"/>
-        <v>6547</v>
+        <v>5239</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>436.89965234581427</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>351.72858916218547</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1816245</v>
+        <v>1508780</v>
       </c>
       <c r="C6" s="2">
         <f ca="1">VLOOKUP(A6,Sheet1!$A$1:$D$6,4,FALSE)*B6</f>
-        <v>1700860.0235294118</v>
+        <v>1382752.4941176472</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93647058823529417</v>
+        <v>0.91647058823529415</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>6356857.5</v>
+        <v>5280730</v>
       </c>
       <c r="F6" s="3">
         <f ca="1">AVERAGE(Sheet1!B6:D6)*E6</f>
-        <v>5494319.1882352941</v>
+        <v>4529002.552941177</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.86431372549019603</v>
+        <v>0.85764705882352954</v>
       </c>
       <c r="H6">
         <f ca="1">RANDBETWEEN(5000,10000)</f>
-        <v>7910</v>
+        <v>5302</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>215.02655164720755</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>260.79828255708168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
@@ -874,22 +879,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD9BC797-0D86-4766-8D83-AAE07F6177DD}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -915,29 +920,29 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2">
         <f ca="1">SUM(B3:B6)</f>
-        <v>6947217.3500000006</v>
+        <v>6456465.1600000001</v>
       </c>
       <c r="C2" s="2">
         <f ca="1">SUM(C3:C6)</f>
-        <v>5907554.5984508451</v>
+        <v>5527807.957108316</v>
       </c>
       <c r="D2" s="1">
         <f ca="1">C2/B2</f>
-        <v>0.85034831945352118</v>
+        <v>0.85616631084063899</v>
       </c>
       <c r="E2">
         <f ca="1">SUM(E3:E6)</f>
-        <v>22144.09</v>
+        <v>22924.199999999997</v>
       </c>
       <c r="F2" s="5">
         <f ca="1">C2/E2</f>
-        <v>266.77793481018392</v>
+        <v>241.13417075005088</v>
       </c>
       <c r="G2" s="4">
         <f>MAX(G3:G6)</f>
@@ -948,29 +953,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2">
         <f ca="1">Sheet2!B3*(1-RANDBETWEEN(5,20)/100)</f>
-        <v>1151348.8</v>
+        <v>877321.92</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">VLOOKUP(A3,Sheet1!$A$1:$D$6,3,FALSE)*B3</f>
-        <v>898052.06400000025</v>
+        <v>684311.0976000001</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D6" ca="1" si="0">C3/B3</f>
-        <v>0.78000000000000014</v>
+        <v>0.78</v>
       </c>
       <c r="E3" s="2">
         <f ca="1">Sheet2!H3*(1-RANDBETWEEN(5,20)/100)</f>
-        <v>5016</v>
+        <v>7391.7</v>
       </c>
       <c r="F3" s="5">
         <f ca="1">C3/E3</f>
-        <v>179.03749282296656</v>
+        <v>92.578310483380022</v>
       </c>
       <c r="G3" s="4">
         <v>44732</v>
@@ -980,29 +985,29 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2">
         <f ca="1">Sheet2!B4*(1-RANDBETWEEN(5,20)/100)</f>
-        <v>1573976.64</v>
+        <v>2543048.64</v>
       </c>
       <c r="C4" s="2">
         <f ca="1">VLOOKUP(A4,Sheet1!$A$1:$D$6,3,FALSE)*B4</f>
-        <v>1385099.4431999999</v>
+        <v>2237882.8032</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88</v>
+        <v>0.87999999999999989</v>
       </c>
       <c r="E4" s="2">
         <f ca="1">Sheet2!H4*(1-RANDBETWEEN(5,20)/100)</f>
-        <v>4907.79</v>
+        <v>6361.2</v>
       </c>
       <c r="F4" s="5">
         <f ca="1">C4/E4</f>
-        <v>282.22467611694873</v>
+        <v>351.80198754951897</v>
       </c>
       <c r="G4" s="4">
         <v>45137</v>
@@ -1012,42 +1017,42 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2">
         <f ca="1">Sheet2!B5*(1-RANDBETWEEN(5,20)/100)</f>
-        <v>2569108.96</v>
+        <v>1602753.6</v>
       </c>
       <c r="C5" s="2">
         <f ca="1">VLOOKUP(A5,Sheet1!$A$1:$D$6,3,FALSE)*B5</f>
-        <v>2208843.1058390806</v>
+        <v>1377999.6468965518</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85977011494252886</v>
+        <v>0.85977011494252875</v>
       </c>
       <c r="E5" s="2">
         <f ca="1">Sheet2!H5*(1-RANDBETWEEN(5,20)/100)</f>
-        <v>5892.3</v>
+        <v>4505.54</v>
       </c>
       <c r="F5" s="5">
         <f ca="1">C5/E5</f>
-        <v>374.86942379700298</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>305.84561382132927</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2">
         <f ca="1">Sheet2!B6*(1-RANDBETWEEN(5,20)/100)</f>
-        <v>1652782.95</v>
+        <v>1433341</v>
       </c>
       <c r="C6" s="2">
         <f ca="1">VLOOKUP(A6,Sheet1!$A$1:$D$6,3,FALSE)*B6</f>
-        <v>1415559.9854117646</v>
+        <v>1227614.4094117647</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1055,11 +1060,11 @@
       </c>
       <c r="E6" s="2">
         <f ca="1">Sheet2!H6*(1-RANDBETWEEN(5,20)/100)</f>
-        <v>6328</v>
+        <v>4665.76</v>
       </c>
       <c r="F6" s="5">
         <f ca="1">C6/E6</f>
-        <v>223.6978485163977</v>
+        <v>263.11134936468329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>